<commit_message>
update code IdentityServer 4
</commit_message>
<xml_diff>
--- a/Document/CI/Account.xlsx
+++ b/Document/CI/Account.xlsx
@@ -755,7 +755,7 @@
   <dimension ref="A3:D26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -843,7 +843,7 @@
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -968,13 +968,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update code IdentityServer 4 for MVC client
</commit_message>
<xml_diff>
--- a/Document/CI/Account.xlsx
+++ b/Document/CI/Account.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Column3</t>
   </si>
@@ -137,6 +137,38 @@
   </si>
   <si>
     <t>root</t>
+  </si>
+  <si>
+    <t>old: Qux80908
+new: Abc@@123HH</t>
+  </si>
+  <si>
+    <t>Power Be Caready</t>
+  </si>
+  <si>
+    <t>Onn-premises data gateway Caready</t>
+  </si>
+  <si>
+    <t>Caready on-premises</t>
+  </si>
+  <si>
+    <t>Caready@@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ci_caready@ciagency.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>Analytics_Data</t>
+  </si>
+  <si>
+    <t>Domain / IP
+103.77.166.113
+Database
+Analytics_Data
+Username
+analytics_read_data_login
+Password
+Nextgroup@1230</t>
   </si>
 </sst>
 </file>
@@ -213,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -236,6 +268,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -754,14 +787,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.81640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.54296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="26.26953125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="2"/>
@@ -891,13 +924,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+    <row r="14" spans="1:4" ht="35" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="35" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
@@ -980,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D4"/>
+  <dimension ref="A3:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -1017,6 +1064,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="112" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>